<commit_message>
Working for Cards filter
</commit_message>
<xml_diff>
--- a/excel/C-卡片配置.xlsx
+++ b/excel/C-卡片配置.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B5910A-B5E6-43C4-AEF2-25BB05324E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2576A6F7-E8E7-4E4D-AD75-C3105CC185E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1483,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1688,7 +1688,7 @@
         <v>3</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -1893,7 +1893,7 @@
         <v>4</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>2</v>
@@ -2098,7 +2098,7 @@
         <v>9</v>
       </c>
       <c r="J23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>2</v>

</xml_diff>